<commit_message>
Improved polish of plot outputs
</commit_message>
<xml_diff>
--- a/Forecast_Model.xlsx
+++ b/Forecast_Model.xlsx
@@ -286,10 +286,10 @@
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G21" activeCellId="0" sqref="G21"/>
+      <selection pane="topLeft" activeCell="D22" activeCellId="0" sqref="D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="13.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.22"/>
@@ -625,7 +625,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">

</xml_diff>